<commit_message>
Supprimer les ValueSet VS-TRE-R74-ModeFixationTarifaire VS-TRE-R286-TypeFermeture VS-TRE-R301-SourceInformationInstallation et utiliser ceux des NOS (J259, J260, J261) (#247)
* rm jdv

* update release notes 5f5b26062127d5d15d311b80817ff76c8cf9ddc5
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-as-dp-healthcareservice-social-equipment.xlsx
+++ b/main/ig/StructureDefinition-as-dp-healthcareservice-social-equipment.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-11-14T08:22:05+00:00</t>
+    <t>2024-11-18T16:15:50+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -992,7 +992,7 @@
     <t>required</t>
   </si>
   <si>
-    <t>https://interop.esante.gouv.fr/ig/fhir/annuaire/ValueSet/VS-TRE-R301-SourceInformationInstallation</t>
+    <t>https://mos.esante.gouv.fr/NOS/JDV_J261-SourceInformationInstallation-RASS/FHIR/JDV-J261-SourceInformationInstallation-RASS</t>
   </si>
   <si>
     <t>HealthcareService.extension:as-ext-installation.url</t>
@@ -2432,7 +2432,7 @@
     <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="98.61328125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="115.26171875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="118.76953125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>

</xml_diff>